<commit_message>
Initial release of GlyQ-IQ automation plugin
</commit_message>
<xml_diff>
--- a/Plugins/AM_GlyQIQ_Plugin/Docs/Parameters.xlsx
+++ b/Plugins/AM_GlyQIQ_Plugin/Docs/Parameters.xlsx
@@ -285,9 +285,6 @@
     <t>GlyQIQ_AppFiles_Master: MgrParams</t>
   </si>
   <si>
-    <t>GlyQIQ_AppFiles_HPC:     Path.combine(udtHPCOptions.WorkDirPath, "GlyQ_ApplicationFiles")</t>
-  </si>
-  <si>
     <t>Sync %GlyQIQ_AppFiles_Master% with %GlyQIQ_AppFiles_HPC%</t>
   </si>
   <si>
@@ -436,6 +433,9 @@
   </si>
   <si>
     <t>Settings File (make sure it ends in .txt)</t>
+  </si>
+  <si>
+    <t>GlyQIQ_AppFiles_HPC:     Path.combine(udtHPCOptions.SharePath, "GlyQ_ApplicationFiles")</t>
   </si>
 </sst>
 </file>
@@ -796,10 +796,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A37" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -822,7 +822,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>65</v>
@@ -854,7 +854,7 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G4" s="1">
         <v>50</v>
@@ -934,10 +934,10 @@
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -954,10 +954,10 @@
         <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -974,7 +974,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>1</v>
@@ -994,7 +994,7 @@
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>4</v>
@@ -1014,7 +1014,7 @@
         <v>31</v>
       </c>
       <c r="F12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>31</v>
@@ -1034,7 +1034,7 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>10</v>
@@ -1054,7 +1054,7 @@
         <v>34</v>
       </c>
       <c r="F14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>34</v>
@@ -1074,7 +1074,7 @@
         <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>36</v>
@@ -1088,7 +1088,7 @@
         <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>12</v>
@@ -1102,7 +1102,7 @@
         <v>38</v>
       </c>
       <c r="F17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>38</v>
@@ -1116,7 +1116,7 @@
         <v>40</v>
       </c>
       <c r="F18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>40</v>
@@ -1130,10 +1130,10 @@
         <v>42</v>
       </c>
       <c r="F19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.3">
@@ -1144,10 +1144,10 @@
         <v>42</v>
       </c>
       <c r="F20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.3">
@@ -1158,7 +1158,7 @@
         <v>28</v>
       </c>
       <c r="F21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.3">
@@ -1169,7 +1169,7 @@
         <v>46</v>
       </c>
       <c r="F22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>46</v>
@@ -1183,7 +1183,7 @@
         <v>55</v>
       </c>
       <c r="F23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>55</v>
@@ -1197,7 +1197,7 @@
         <v>18</v>
       </c>
       <c r="F24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>18</v>
@@ -1211,10 +1211,10 @@
         <v>55</v>
       </c>
       <c r="F25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.3">
@@ -1225,7 +1225,7 @@
         <v>51</v>
       </c>
       <c r="F26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>51</v>
@@ -1239,7 +1239,7 @@
         <v>53</v>
       </c>
       <c r="F27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>53</v>
@@ -1253,7 +1253,7 @@
         <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G28" s="1">
         <v>1170</v>
@@ -1310,7 +1310,7 @@
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E36" t="s">
-        <v>89</v>
+        <v>139</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>60</v>
@@ -1324,7 +1324,7 @@
         <v>69</v>
       </c>
       <c r="E37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F37" s="3"/>
     </row>
@@ -1341,7 +1341,7 @@
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.3">
@@ -1349,32 +1349,32 @@
         <v>3</v>
       </c>
       <c r="D41" t="s">
+        <v>122</v>
+      </c>
+      <c r="E41" t="s">
         <v>123</v>
       </c>
-      <c r="E41" t="s">
-        <v>124</v>
-      </c>
       <c r="F41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
+        <v>131</v>
+      </c>
+      <c r="E42" t="s">
+        <v>124</v>
+      </c>
+      <c r="F42" t="s">
         <v>132</v>
-      </c>
-      <c r="E42" t="s">
-        <v>125</v>
-      </c>
-      <c r="F42" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="3:6" x14ac:dyDescent="0.3">
@@ -1387,34 +1387,34 @@
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E45" t="s">
+        <v>126</v>
+      </c>
+      <c r="F45" t="s">
         <v>127</v>
-      </c>
-      <c r="F45" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E47" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F47" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.3">
@@ -1425,12 +1425,12 @@
         <v>70</v>
       </c>
       <c r="E51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E52" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.3">
@@ -1450,42 +1450,42 @@
     </row>
     <row r="56" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E56" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E60" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E63" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="64" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="66" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E66" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="68" spans="3:5" x14ac:dyDescent="0.3">
@@ -1496,7 +1496,7 @@
         <v>66</v>
       </c>
       <c r="E68" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="70" spans="3:5" x14ac:dyDescent="0.3">
@@ -1515,20 +1515,20 @@
         <v>7</v>
       </c>
       <c r="D72" t="s">
+        <v>110</v>
+      </c>
+      <c r="E72" t="s">
         <v>111</v>
-      </c>
-      <c r="E72" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="73" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E73" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="74" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E74" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>